<commit_message>
Updated Order sheet & BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ringl\Documents\Uni Classes\Y3S2\EE318-Project\EE318-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9E4D54-64EE-42BA-AB7D-F3C390367F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D946BF9-7C2F-4366-A34E-25180F1A2CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12377" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
   <si>
     <t>Part No</t>
   </si>
@@ -123,13 +123,88 @@
   </si>
   <si>
     <t>Total Price</t>
+  </si>
+  <si>
+    <t>Seeed Studio</t>
+  </si>
+  <si>
+    <t>179-3740</t>
+  </si>
+  <si>
+    <t>0.5W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://uk.rs-online.com/web/p/stem-motion-components/2153180 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://uk.rs-online.com/web/p/solar-panels/1793740 </t>
+  </si>
+  <si>
+    <t>Kitronik</t>
+  </si>
+  <si>
+    <t>215-3180</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>from lab?</t>
+  </si>
+  <si>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>Yellow/Orange LED</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>Push Buttons</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>MSP430 LaunchPad</t>
+  </si>
+  <si>
+    <t>Resource Centre</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>10k resistor</t>
+  </si>
+  <si>
+    <t>1k Resistor</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>From Workshop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +216,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,20 +249,189 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="12">
     <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
@@ -197,22 +448,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86A91721-DFC9-4530-9507-923262E7E515}" name="Table3" displayName="Table3" ref="A1:K8" insertRowShift="1" totalsRowShown="0">
-  <autoFilter ref="A1:K8" xr:uid="{86A91721-DFC9-4530-9507-923262E7E515}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86A91721-DFC9-4530-9507-923262E7E515}" name="Table3" displayName="Table3" ref="A1:K16" insertRowShift="1" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:K16" xr:uid="{86A91721-DFC9-4530-9507-923262E7E515}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{ECA0EC40-399A-4C70-978E-42FB9C151DEF}" name="Part No" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{F559D445-4E6C-49CD-BE56-D45174266346}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{08B644CF-697F-4D1E-A082-11CDE9ED0629}" name="Quantity"/>
-    <tableColumn id="4" xr3:uid="{D142A8D3-BBEC-4CEC-AF0E-C8DDB745BB0B}" name="Manufacturer"/>
-    <tableColumn id="5" xr3:uid="{BF69BCDB-F77E-4978-A85F-E82361F31AB3}" name="Manufacturer Part Number"/>
-    <tableColumn id="6" xr3:uid="{6F64C4FD-3D82-4B97-91BA-EBFF5FA86E4E}" name="Supplier"/>
-    <tableColumn id="9" xr3:uid="{54E86A7E-C3AE-4ED4-BED8-641F8DD43B4E}" name="Supplier Part Number"/>
-    <tableColumn id="7" xr3:uid="{23C8AAEA-D529-4A7F-A9DA-8264FA5C0044}" name="Value"/>
-    <tableColumn id="10" xr3:uid="{2768BD98-C717-4B84-9AC1-B93A7F458DEA}" name="Price"/>
-    <tableColumn id="11" xr3:uid="{17F0A9B8-6879-45C1-9BB1-AC84DBF4B1D8}" name="Total Price" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{ECA0EC40-399A-4C70-978E-42FB9C151DEF}" name="Part No" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{F559D445-4E6C-49CD-BE56-D45174266346}" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{08B644CF-697F-4D1E-A082-11CDE9ED0629}" name="Quantity" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{D142A8D3-BBEC-4CEC-AF0E-C8DDB745BB0B}" name="Manufacturer" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{BF69BCDB-F77E-4978-A85F-E82361F31AB3}" name="Manufacturer Part Number" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{6F64C4FD-3D82-4B97-91BA-EBFF5FA86E4E}" name="Supplier" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{54E86A7E-C3AE-4ED4-BED8-641F8DD43B4E}" name="Supplier Part Number" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{23C8AAEA-D529-4A7F-A9DA-8264FA5C0044}" name="Value" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{2768BD98-C717-4B84-9AC1-B93A7F458DEA}" name="Price" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{17F0A9B8-6879-45C1-9BB1-AC84DBF4B1D8}" name="Total Price" dataDxfId="7">
       <calculatedColumnFormula>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5422AE89-5DBF-4BA2-9E9F-B7B90C91198F}" name="Link"/>
+    <tableColumn id="8" xr3:uid="{5422AE89-5DBF-4BA2-9E9F-B7B90C91198F}" name="Link" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -481,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -539,65 +790,105 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="J2">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="6">
+        <v>313070004</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="J2" s="2">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>3.6</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="J3">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
+      <c r="D3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2565</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="J3" s="2">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>4.2</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>0.95</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
         <v>0.95</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -605,58 +896,323 @@
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="J5">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
+      <c r="D5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="J6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J7">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J8">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="5">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="5">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="5">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="5">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="5">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19">
+        <f>SUM(Table3[Total Price])</f>
+        <v>8.75</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K4" r:id="rId1" xr:uid="{B2D61BB8-2751-4A49-9A37-1930750871E3}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{7D3F2FEE-159A-41C0-9D52-5434B792AC02}"/>
+    <hyperlink ref="K2" r:id="rId3" xr:uid="{D679E73D-7666-4DB4-AFE5-DB4FDAF108AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated code. Added light rail basic CAD. added PCB
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ringl\Documents\Uni Classes\Y3S2\EE318-Project\EE318-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D946BF9-7C2F-4366-A34E-25180F1A2CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCE05DF-1DFB-466B-AB37-14C0B452DC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12377" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t>Part No</t>
   </si>
@@ -89,9 +89,6 @@
     <t>LDR</t>
   </si>
   <si>
-    <t>3-8 Multiplexer</t>
-  </si>
-  <si>
     <t>https://uk.rs-online.com/web/p/potentiometers/8274990</t>
   </si>
   <si>
@@ -198,6 +195,21 @@
   </si>
   <si>
     <t>From Workshop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://uk.rs-online.com/web/p/multiplexer-demultiplexer-ics/0580856 </t>
+  </si>
+  <si>
+    <t>Toshiba</t>
+  </si>
+  <si>
+    <t>580-856</t>
+  </si>
+  <si>
+    <t>TC4051BP</t>
+  </si>
+  <si>
+    <t>1-8 Multiplexer</t>
   </si>
 </sst>
 </file>
@@ -249,22 +261,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -285,7 +295,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -299,6 +308,47 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -379,7 +429,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -393,46 +443,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -448,22 +458,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86A91721-DFC9-4530-9507-923262E7E515}" name="Table3" displayName="Table3" ref="A1:K16" insertRowShift="1" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86A91721-DFC9-4530-9507-923262E7E515}" name="Table3" displayName="Table3" ref="A1:K16" insertRowShift="1" totalsRowShown="0" dataDxfId="11">
   <autoFilter ref="A1:K16" xr:uid="{86A91721-DFC9-4530-9507-923262E7E515}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{ECA0EC40-399A-4C70-978E-42FB9C151DEF}" name="Part No" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{F559D445-4E6C-49CD-BE56-D45174266346}" name="Name" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{08B644CF-697F-4D1E-A082-11CDE9ED0629}" name="Quantity" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{D142A8D3-BBEC-4CEC-AF0E-C8DDB745BB0B}" name="Manufacturer" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{BF69BCDB-F77E-4978-A85F-E82361F31AB3}" name="Manufacturer Part Number" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{6F64C4FD-3D82-4B97-91BA-EBFF5FA86E4E}" name="Supplier" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{54E86A7E-C3AE-4ED4-BED8-641F8DD43B4E}" name="Supplier Part Number" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{23C8AAEA-D529-4A7F-A9DA-8264FA5C0044}" name="Value" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{2768BD98-C717-4B84-9AC1-B93A7F458DEA}" name="Price" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{17F0A9B8-6879-45C1-9BB1-AC84DBF4B1D8}" name="Total Price" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{ECA0EC40-399A-4C70-978E-42FB9C151DEF}" name="Part No" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{F559D445-4E6C-49CD-BE56-D45174266346}" name="Name" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{08B644CF-697F-4D1E-A082-11CDE9ED0629}" name="Quantity" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{D142A8D3-BBEC-4CEC-AF0E-C8DDB745BB0B}" name="Manufacturer" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{BF69BCDB-F77E-4978-A85F-E82361F31AB3}" name="Manufacturer Part Number" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{6F64C4FD-3D82-4B97-91BA-EBFF5FA86E4E}" name="Supplier" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{54E86A7E-C3AE-4ED4-BED8-641F8DD43B4E}" name="Supplier Part Number" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{23C8AAEA-D529-4A7F-A9DA-8264FA5C0044}" name="Value" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{2768BD98-C717-4B84-9AC1-B93A7F458DEA}" name="Price" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{17F0A9B8-6879-45C1-9BB1-AC84DBF4B1D8}" name="Total Price" dataDxfId="1">
       <calculatedColumnFormula>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5422AE89-5DBF-4BA2-9E9F-B7B90C91198F}" name="Link" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{5422AE89-5DBF-4BA2-9E9F-B7B90C91198F}" name="Link" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -735,12 +745,12 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="19.07421875" customWidth="1"/>
+    <col min="2" max="2" width="23.07421875" customWidth="1"/>
     <col min="3" max="3" width="10.07421875" customWidth="1"/>
     <col min="4" max="4" width="18.765625" customWidth="1"/>
     <col min="5" max="5" width="25.15234375" customWidth="1"/>
@@ -771,436 +781,415 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="4">
+        <v>313070004</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="6">
-        <v>313070004</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="I2">
         <v>3.6</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
         <v>3.6</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>33</v>
+      <c r="K2" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2565</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="6">
-        <v>2565</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2">
+      <c r="I3">
         <v>4.2</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
         <v>4.2</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>32</v>
+      <c r="K3" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="2">
+      <c r="I4">
         <v>0.95</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
         <v>0.95</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>18</v>
+      <c r="K4" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="2"/>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="J5">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="2"/>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="J6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>2.665</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="2"/>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="2"/>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="5">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="2"/>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="J10">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="5">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="2"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="J11">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="2">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="2"/>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>3</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="5">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="7"/>
+      <c r="E13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="5">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="2"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="J14">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="5">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="2"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="J15">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="5">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="2"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="J16">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="9:10" x14ac:dyDescent="0.4">
       <c r="I19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J19">
         <f>SUM(Table3[Total Price])</f>
-        <v>8.75</v>
+        <v>11.414999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1208,11 +1197,12 @@
     <hyperlink ref="K4" r:id="rId1" xr:uid="{B2D61BB8-2751-4A49-9A37-1930750871E3}"/>
     <hyperlink ref="K3" r:id="rId2" xr:uid="{7D3F2FEE-159A-41C0-9D52-5434B792AC02}"/>
     <hyperlink ref="K2" r:id="rId3" xr:uid="{D679E73D-7666-4DB4-AFE5-DB4FDAF108AA}"/>
+    <hyperlink ref="K6" r:id="rId4" xr:uid="{A60C7C60-8B20-4741-B1EB-B281AA7E0190}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>